<commit_message>
Addition of calc of rxn force due to oxidizer mass flux
</commit_message>
<xml_diff>
--- a/FlowRateCalcs_BJ01_Oxidizer.xlsx
+++ b/FlowRateCalcs_BJ01_Oxidizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD Documents\Propulsion Github\Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD63CCDB-98D7-4317-92B8-7B01E35A71A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BF7A5A-240A-4F36-A5D2-CB2503EB2276}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15540" xr2:uid="{31DEBCDE-38FC-CA4F-B845-A280DAD82E45}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Flow Rate Calculations for BJ-01 Oxidizer System</t>
   </si>
@@ -87,9 +87,6 @@
     <t>OUTUTS</t>
   </si>
   <si>
-    <t>Run Tan Outputs</t>
-  </si>
-  <si>
     <t>System Outputs</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>RT out/plumb in. threading</t>
   </si>
   <si>
-    <t>ESTIMATED guess of Pressure drop across injector (psi)</t>
-  </si>
-  <si>
     <t>ASSUMES Pressure at injector inlet = P_combch. + P_estimated drop across injector plate</t>
   </si>
   <si>
@@ -172,14 +166,53 @@
   </si>
   <si>
     <t>1/2" dia</t>
+  </si>
+  <si>
+    <t>Run Tank Outputs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ACaslonPro-Regular"/>
+      </rPr>
+      <t>ESTIMATED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ACaslonPro-Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> guess of Pressure drop across injector (psi)</t>
+    </r>
+  </si>
+  <si>
+    <t>Flow Velocity (in/s)</t>
+  </si>
+  <si>
+    <t>Force of Mass Flux (lbf)</t>
+  </si>
+  <si>
+    <t>Min. Inner Pipe Radius (in)</t>
+  </si>
+  <si>
+    <t>Min. Inner Pipe Area (in^2)</t>
+  </si>
+  <si>
+    <t>Maximum, worst case reaction force on RT caused by mass flow rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -270,7 +303,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -393,11 +426,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -452,14 +507,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -483,6 +532,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,7 +873,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -809,21 +881,22 @@
     <col min="1" max="1" width="36.875" customWidth="1"/>
     <col min="2" max="2" width="45.875" customWidth="1"/>
     <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="19.375" customWidth="1"/>
+    <col min="6" max="6" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="39"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="B3" s="8"/>
@@ -847,13 +920,13 @@
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="21" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="17">
         <v>815</v>
@@ -890,7 +963,7 @@
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="10"/>
     </row>
@@ -911,13 +984,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="17">
         <v>0</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="4">
         <f>C6-(C11+C16)</f>
@@ -926,80 +999,105 @@
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="24">
         <v>0.51680000000000004</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="D13" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="43">
         <f>SUM(C18:C21)</f>
         <v>1.53</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="14">
         <v>2.683845E-2</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="4"/>
+      <c r="D14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="41">
+        <f>(E20/2)</f>
+        <v>0.13072203530776505</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="27"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="14">
         <v>386.08858300000003</v>
       </c>
-      <c r="D15" s="19"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="27"/>
-      <c r="B16" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="14">
+      <c r="D15" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15">
+        <f>PI()*(E14^2)</f>
+        <v>5.3684322280640365E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15">
+      <c r="A16" s="38"/>
+      <c r="B16" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="16">
         <v>100</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16">
+        <f>C13/(C14*E15)</f>
+        <v>358.68862124652077</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
-      <c r="A17" s="26" t="s">
-        <v>39</v>
+      <c r="A17" s="39" t="s">
+        <v>38</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="16"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
+      <c r="D17" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="46">
+        <f>C13*E16/12</f>
+        <v>15.447523288350162</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>53</v>
+      </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="24">
         <v>0.5</v>
       </c>
-      <c r="D18" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="29"/>
+      <c r="D18" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="27"/>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="4">
         <f>E13+1</f>
@@ -1008,18 +1106,18 @@
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1">
       <c r="A19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>41</v>
       </c>
       <c r="C19" s="24">
         <v>0.08</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="29"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="27"/>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G19">
         <f>((1/C7)^4)</f>
@@ -1028,7 +1126,7 @@
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>16</v>
@@ -1036,13 +1134,13 @@
       <c r="C20" s="24">
         <v>0.05</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="29">
+      <c r="D20" s="35"/>
+      <c r="E20" s="27">
         <f>(G18/(G19+G20))^(1/4)</f>
         <v>0.2614440706155301</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20">
         <f>(0.25*((C14*PI()/C13)^2)*(((E12*12)/C14)+(C15*E11)))</f>
@@ -1051,7 +1149,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -1059,35 +1157,35 @@
       <c r="C21" s="24">
         <v>0.9</v>
       </c>
-      <c r="D21" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="33">
+      <c r="D21" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="31">
         <v>1.75</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15">
       <c r="C22" s="14"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="30">
+      <c r="E22" s="28">
         <f>E21*E20</f>
         <v>0.45752712357717767</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="C23" s="14"/>
-      <c r="D23" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>48</v>
+      <c r="D23" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1">
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickTop="1">
       <c r="B25" s="3" t="s">
@@ -1118,13 +1216,13 @@
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" thickBot="1">
+      <c r="B30" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1">
-      <c r="B30" s="32" t="s">
-        <v>45</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1142,7 +1240,7 @@
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1152,6 +1250,6 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>